<commit_message>
made some changes but meh
</commit_message>
<xml_diff>
--- a/csv_data/ORI_IDs.xlsx
+++ b/csv_data/ORI_IDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\jamie\Documents\school\DATA ANALYTICS\project_shit\proj1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\Documents\School\Data Analytics\Projects\proj1\csv_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEC7AF40-6A03-4A04-B1D4-F5973DF3FBDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E443495-901A-4D35-ADA4-C88E546A9D88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{C7C16CA1-BC7B-4FFB-825B-F92A5DFD81E6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C7C16CA1-BC7B-4FFB-825B-F92A5DFD81E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="302">
   <si>
     <t>TX1010000</t>
   </si>
@@ -394,18 +394,6 @@
   </si>
   <si>
     <t>SCHOOL DISTRICT PD</t>
-  </si>
-  <si>
-    <t>TX1013600</t>
-  </si>
-  <si>
-    <t>SAN JACINTO COLLEGE CENTRAL CAMPUS PD PASADENA</t>
-  </si>
-  <si>
-    <t>SAN JACINTO COLLEGE</t>
-  </si>
-  <si>
-    <t>CENTRAL CAMPUS PD</t>
   </si>
   <si>
     <t>TX1013700</t>
@@ -1335,24 +1323,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA21F29-11BD-439B-82F9-4574E16DC1A0}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1398,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1421,7 +1409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1444,7 +1432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1467,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1490,7 +1478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1513,7 +1501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1536,7 +1524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1559,7 +1547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1582,7 +1570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -1605,7 +1593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -1628,7 +1616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1651,7 +1639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1674,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1697,7 +1685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -1720,7 +1708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1743,7 +1731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1766,7 +1754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1789,7 +1777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -1812,7 +1800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
@@ -1835,7 +1823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
@@ -1858,7 +1846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
@@ -1881,7 +1869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -1904,7 +1892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -1927,7 +1915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -1950,7 +1938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
@@ -1973,7 +1961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -1996,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
@@ -2019,7 +2007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
@@ -2042,7 +2030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>89</v>
       </c>
@@ -2065,7 +2053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
@@ -2088,7 +2076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
@@ -2111,7 +2099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>96</v>
       </c>
@@ -2134,7 +2122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>99</v>
       </c>
@@ -2157,7 +2145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>103</v>
       </c>
@@ -2180,7 +2168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>106</v>
       </c>
@@ -2203,7 +2191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>109</v>
       </c>
@@ -2226,7 +2214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
@@ -2249,7 +2237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
@@ -2272,7 +2260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -2280,68 +2268,68 @@
         <v>122</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="F41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>131</v>
       </c>
@@ -2355,7 +2343,7 @@
         <v>134</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>102</v>
@@ -2364,7 +2352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>135</v>
       </c>
@@ -2375,73 +2363,73 @@
         <v>137</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="G46" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>147</v>
+        <v>29</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>148</v>
@@ -2456,7 +2444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>150</v>
       </c>
@@ -2479,7 +2467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>154</v>
       </c>
@@ -2502,7 +2490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>158</v>
       </c>
@@ -2516,27 +2504,27 @@
         <v>160</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>21</v>
@@ -2548,18 +2536,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>21</v>
@@ -2571,18 +2559,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>21</v>
@@ -2594,30 +2582,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>173</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
@@ -2628,42 +2616,42 @@
         <v>176</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E57" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>181</v>
       </c>
@@ -2680,13 +2668,13 @@
         <v>3</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>185</v>
       </c>
@@ -2697,42 +2685,42 @@
         <v>187</v>
       </c>
       <c r="D59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E60" s="1" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>192</v>
       </c>
@@ -2746,62 +2734,62 @@
         <v>195</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="E62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E63" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>204</v>
       </c>
@@ -2818,13 +2806,13 @@
         <v>3</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>208</v>
       </c>
@@ -2832,34 +2820,34 @@
         <v>209</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E66" s="1" t="s">
         <v>3</v>
       </c>
@@ -2870,7 +2858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>214</v>
       </c>
@@ -2893,7 +2881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>218</v>
       </c>
@@ -2904,42 +2892,42 @@
         <v>220</v>
       </c>
       <c r="D68" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E69" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>225</v>
       </c>
@@ -2950,88 +2938,88 @@
         <v>227</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="D72" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="C73" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="F73" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>238</v>
       </c>
@@ -3039,80 +3027,80 @@
         <v>239</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="E75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="E77" s="1" t="s">
         <v>3</v>
       </c>
@@ -3123,7 +3111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>253</v>
       </c>
@@ -3134,31 +3122,31 @@
         <v>255</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="E79" s="1" t="s">
         <v>3</v>
       </c>
@@ -3169,7 +3157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>260</v>
       </c>
@@ -3192,7 +3180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>264</v>
       </c>
@@ -3206,16 +3194,16 @@
         <v>267</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>268</v>
       </c>
@@ -3229,16 +3217,16 @@
         <v>271</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>272</v>
       </c>
@@ -3249,31 +3237,31 @@
         <v>274</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="E84" s="1" t="s">
         <v>3</v>
       </c>
@@ -3284,7 +3272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>279</v>
       </c>
@@ -3295,56 +3283,56 @@
         <v>281</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="E86" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>8</v>
+        <v>286</v>
+      </c>
+      <c r="F86" s="2">
+        <v>3</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>290</v>
+        <v>16</v>
       </c>
       <c r="F87" s="2">
         <v>3</v>
@@ -3353,7 +3341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>291</v>
       </c>
@@ -3364,19 +3352,19 @@
         <v>293</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F88" s="2">
-        <v>3</v>
+      <c r="F88" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>295</v>
       </c>
@@ -3387,19 +3375,19 @@
         <v>297</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>29</v>
+        <v>298</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>298</v>
+        <v>3</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>299</v>
       </c>
@@ -3407,11 +3395,11 @@
         <v>300</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="E90" s="1" t="s">
         <v>3</v>
       </c>
@@ -3419,29 +3407,6 @@
         <v>8</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G91" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>